<commit_message>
atualizando arquivos excel e Power BI
</commit_message>
<xml_diff>
--- a/Curso Excel Básico ao Avançado/Pasta (1).xlsx
+++ b/Curso Excel Básico ao Avançado/Pasta (1).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{096A81CD-4DD9-49A5-A2DE-851BF5DBA79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E7916D1-9714-4D7B-837C-951837B9DCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,11 +129,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,15 +467,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="5" spans="2:8">
       <c r="B5" s="1" t="s">
@@ -556,7 +556,7 @@
       <c r="D8">
         <v>110.5</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F8">

</xml_diff>